<commit_message>
update changes: register and ubicacion service
</commit_message>
<xml_diff>
--- a/utils/data.xlsx
+++ b/utils/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vagot\Documents\GitHub\UNMSM\DSW\PROYECTO_SISVITA\sisvita-backend\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0988A06-80F0-4529-BC8E-B1AEF42E3BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A62D27-8A7D-4915-BA26-3EF8193BABF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B1315F33-F4C0-4336-ADCE-7DD268B96EDD}"/>
   </bookViews>
@@ -1108,6 +1108,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1160,7 +1163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1169,7 +1172,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1486,22 +1490,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{507724CA-D492-4699-B9D4-755E962D55B1}">
   <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="4"/>
+    <col min="2" max="2" width="28.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>355</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1515,16 +1522,16 @@
       <c r="A2" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="5">
         <v>-12.0603</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="5">
         <v>-77.149199999999993</v>
       </c>
     </row>
@@ -1532,16 +1539,16 @@
       <c r="A3" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="5">
         <v>-12.0625</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="5">
         <v>-77.131699999999995</v>
       </c>
     </row>
@@ -1549,16 +1556,16 @@
       <c r="A4" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="5">
         <v>-12.046099999999999</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="5">
         <v>-77.096900000000005</v>
       </c>
     </row>
@@ -1566,16 +1573,16 @@
       <c r="A5" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="5">
         <v>-12.071099999999999</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="5">
         <v>-77.121099999999998</v>
       </c>
     </row>
@@ -1583,16 +1590,16 @@
       <c r="A6" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="5">
         <v>-12.0717</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="5">
         <v>-77.169200000000004</v>
       </c>
     </row>
@@ -1600,16 +1607,16 @@
       <c r="A7" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="5">
         <v>-11.898899999999999</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="5">
         <v>-77.142200000000003</v>
       </c>
     </row>
@@ -1617,16 +1624,16 @@
       <c r="A8" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="5">
         <v>-11.855</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="5">
         <v>-77.125</v>
       </c>
     </row>
@@ -1634,16 +1641,16 @@
       <c r="A9" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="5">
         <v>-12.0467</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="5">
         <v>-77.032200000000003</v>
       </c>
     </row>
@@ -1651,16 +1658,16 @@
       <c r="A10" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="5">
         <v>-11.776400000000001</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="5">
         <v>-77.170299999999997</v>
       </c>
     </row>
@@ -1668,16 +1675,16 @@
       <c r="A11" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="5">
         <v>-12.025600000000001</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="5">
         <v>-76.924199999999999</v>
       </c>
     </row>
@@ -1685,16 +1692,16 @@
       <c r="A12" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="5">
         <v>-12.1494</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="5">
         <v>-77.024699999999996</v>
       </c>
     </row>
@@ -1702,16 +1709,16 @@
       <c r="A13" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="5">
         <v>-12.056699999999999</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="5">
         <v>-77.053600000000003</v>
       </c>
     </row>
@@ -1719,16 +1726,16 @@
       <c r="A14" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="5">
         <v>-11.8583</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="5">
         <v>-77.041899999999998</v>
       </c>
     </row>
@@ -1736,16 +1743,16 @@
       <c r="A15" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="5">
         <v>-11.978300000000001</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="5">
         <v>-76.764200000000002</v>
       </c>
     </row>
@@ -1753,16 +1760,16 @@
       <c r="A16" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="5">
         <v>-12.174200000000001</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="5">
         <v>-77.024699999999996</v>
       </c>
     </row>
@@ -1770,16 +1777,16 @@
       <c r="A17" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="5">
         <v>-12.117800000000001</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="5">
         <v>-76.8125</v>
       </c>
     </row>
@@ -1787,16 +1794,16 @@
       <c r="A18" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="5">
         <v>-11.95</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="5">
         <v>-77.05</v>
       </c>
     </row>
@@ -1804,16 +1811,16 @@
       <c r="A19" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="5">
         <v>-12.0433</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="5">
         <v>-76.998599999999996</v>
       </c>
     </row>
@@ -1821,16 +1828,16 @@
       <c r="A20" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="5">
         <v>-12.0008</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="5">
         <v>-77.052199999999999</v>
       </c>
     </row>
@@ -1838,16 +1845,16 @@
       <c r="A21" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="5">
         <v>-12.069699999999999</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="5">
         <v>-77.045000000000002</v>
       </c>
     </row>
@@ -1855,16 +1862,16 @@
       <c r="A22" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="5">
         <v>-12.0875</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="5">
         <v>-76.933899999999994</v>
       </c>
     </row>
@@ -1872,16 +1879,16 @@
       <c r="A23" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="5">
         <v>-12.065300000000001</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="5">
         <v>-77.030799999999999</v>
       </c>
     </row>
@@ -1889,16 +1896,16 @@
       <c r="A24" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="5">
         <v>-12.081099999999999</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="5">
         <v>-77.030600000000007</v>
       </c>
     </row>
@@ -1906,16 +1913,16 @@
       <c r="A25" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="5">
         <v>-11.982799999999999</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="5">
         <v>-77.069400000000002</v>
       </c>
     </row>
@@ -1923,16 +1930,16 @@
       <c r="A26" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="5">
         <v>-11.937200000000001</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="5">
         <v>-76.703599999999994</v>
       </c>
     </row>
@@ -1940,16 +1947,16 @@
       <c r="A27" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="5">
         <v>-12.268599999999999</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="5">
         <v>-76.884699999999995</v>
       </c>
     </row>
@@ -1957,16 +1964,16 @@
       <c r="A28" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="5">
         <v>-12.0967</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="5">
         <v>-77.074700000000007</v>
       </c>
     </row>
@@ -1974,16 +1981,16 @@
       <c r="A29" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="5">
         <v>-12.0733</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="5">
         <v>-77.063100000000006</v>
       </c>
     </row>
@@ -1991,16 +1998,16 @@
       <c r="A30" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="5">
         <v>-12.1175</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="5">
         <v>-77.045299999999997</v>
       </c>
     </row>
@@ -2008,16 +2015,16 @@
       <c r="A31" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="5">
         <v>-12.2286</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="5">
         <v>-76.859700000000004</v>
       </c>
     </row>
@@ -2025,16 +2032,16 @@
       <c r="A32" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="5">
         <v>-12.4825</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="5">
         <v>-76.796400000000006</v>
       </c>
     </row>
@@ -2042,16 +2049,16 @@
       <c r="A33" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="5">
         <v>-11.846399999999999</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="5">
         <v>-77.105800000000002</v>
       </c>
     </row>
@@ -2059,16 +2066,16 @@
       <c r="A34" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="5">
         <v>-12.3375</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="5">
         <v>-76.825800000000001</v>
       </c>
     </row>
@@ -2076,16 +2083,16 @@
       <c r="A35" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="5">
         <v>-12.366099999999999</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="5">
         <v>-76.794700000000006</v>
       </c>
     </row>
@@ -2093,16 +2100,16 @@
       <c r="A36" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="5">
         <v>-12.029400000000001</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="5">
         <v>-77.043599999999998</v>
       </c>
     </row>
@@ -2110,16 +2117,16 @@
       <c r="A37" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="5">
         <v>-12.388299999999999</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="5">
         <v>-76.780600000000007</v>
       </c>
     </row>
@@ -2127,16 +2134,16 @@
       <c r="A38" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D38" s="4">
+      <c r="D38" s="5">
         <v>-12.107799999999999</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="5">
         <v>-76.998900000000006</v>
       </c>
     </row>
@@ -2144,16 +2151,16 @@
       <c r="A39" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D39" s="5">
         <v>-12.0989</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="5">
         <v>-77.034400000000005</v>
       </c>
     </row>
@@ -2161,16 +2168,16 @@
       <c r="A40" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D40" s="5">
         <v>-12.0244</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="5">
         <v>-77.002499999999998</v>
       </c>
     </row>
@@ -2178,16 +2185,16 @@
       <c r="A41" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D41" s="5">
         <v>-12.158899999999999</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E41" s="5">
         <v>-76.972200000000001</v>
       </c>
     </row>
@@ -2195,16 +2202,16 @@
       <c r="A42" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D42" s="5">
         <v>-12.072800000000001</v>
       </c>
-      <c r="E42" s="4">
+      <c r="E42" s="5">
         <v>-76.997500000000002</v>
       </c>
     </row>
@@ -2212,16 +2219,16 @@
       <c r="A43" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D43" s="5">
         <v>-12.0303</v>
       </c>
-      <c r="E43" s="4">
+      <c r="E43" s="5">
         <v>-77.046899999999994</v>
       </c>
     </row>
@@ -2229,16 +2236,16 @@
       <c r="A44" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D44" s="5">
         <v>-12.09</v>
       </c>
-      <c r="E44" s="4">
+      <c r="E44" s="5">
         <v>-77.086399999999998</v>
       </c>
     </row>
@@ -2246,16 +2253,16 @@
       <c r="A45" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D45" s="5">
         <v>-12.0433</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E45" s="5">
         <v>-76.984999999999999</v>
       </c>
     </row>
@@ -2263,16 +2270,16 @@
       <c r="A46" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D46" s="5">
         <v>-12.4092</v>
       </c>
-      <c r="E46" s="4">
+      <c r="E46" s="5">
         <v>-76.775800000000004</v>
       </c>
     </row>
@@ -2280,16 +2287,16 @@
       <c r="A47" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D47" s="5">
         <v>-11.798299999999999</v>
       </c>
-      <c r="E47" s="4">
+      <c r="E47" s="5">
         <v>-77.177499999999995</v>
       </c>
     </row>
@@ -2297,16 +2304,16 @@
       <c r="A48" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D48" s="5">
         <v>-12.150600000000001</v>
       </c>
-      <c r="E48" s="4">
+      <c r="E48" s="5">
         <v>-77.007800000000003</v>
       </c>
     </row>
@@ -2314,16 +2321,16 @@
       <c r="A49" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D49" s="4">
+      <c r="D49" s="5">
         <v>-12.1136</v>
       </c>
-      <c r="E49" s="4">
+      <c r="E49" s="5">
         <v>-77.008099999999999</v>
       </c>
     </row>
@@ -2331,16 +2338,16 @@
       <c r="A50" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D50" s="4">
+      <c r="D50" s="5">
         <v>-12.2164</v>
       </c>
-      <c r="E50" s="4">
+      <c r="E50" s="5">
         <v>-76.943299999999994</v>
       </c>
     </row>
@@ -2348,16 +2355,16 @@
       <c r="A51" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D51" s="4">
+      <c r="D51" s="5">
         <v>-12.1572</v>
       </c>
-      <c r="E51" s="4">
+      <c r="E51" s="5">
         <v>-76.952799999999996</v>
       </c>
     </row>
@@ -2365,16 +2372,16 @@
       <c r="A52" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D52" s="5">
         <v>-10.756399999999999</v>
       </c>
-      <c r="E52" s="4">
+      <c r="E52" s="5">
         <v>-77.760300000000001</v>
       </c>
     </row>
@@ -2382,16 +2389,16 @@
       <c r="A53" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D53" s="4">
+      <c r="D53" s="5">
         <v>-10.674200000000001</v>
       </c>
-      <c r="E53" s="4">
+      <c r="E53" s="5">
         <v>-77.819699999999997</v>
       </c>
     </row>
@@ -2399,16 +2406,16 @@
       <c r="A54" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D54" s="4">
+      <c r="D54" s="5">
         <v>-10.696099999999999</v>
       </c>
-      <c r="E54" s="4">
+      <c r="E54" s="5">
         <v>-77.779200000000003</v>
       </c>
     </row>
@@ -2416,16 +2423,16 @@
       <c r="A55" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D55" s="4">
+      <c r="D55" s="5">
         <v>-10.799200000000001</v>
       </c>
-      <c r="E55" s="4">
+      <c r="E55" s="5">
         <v>-77.713300000000004</v>
       </c>
     </row>
@@ -2433,16 +2440,16 @@
       <c r="A56" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D56" s="4">
+      <c r="D56" s="5">
         <v>-10.8003</v>
       </c>
-      <c r="E56" s="4">
+      <c r="E56" s="5">
         <v>-77.744699999999995</v>
       </c>
     </row>
@@ -2450,16 +2457,16 @@
       <c r="A57" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D57" s="4">
+      <c r="D57" s="5">
         <v>-10.472200000000001</v>
       </c>
-      <c r="E57" s="4">
+      <c r="E57" s="5">
         <v>-76.993899999999996</v>
       </c>
     </row>
@@ -2467,16 +2474,16 @@
       <c r="A58" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D58" s="4">
+      <c r="D58" s="5">
         <v>-10.3856</v>
       </c>
-      <c r="E58" s="4">
+      <c r="E58" s="5">
         <v>-77.078900000000004</v>
       </c>
     </row>
@@ -2484,16 +2491,16 @@
       <c r="A59" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D59" s="4">
+      <c r="D59" s="5">
         <v>-10.6214</v>
       </c>
-      <c r="E59" s="4">
+      <c r="E59" s="5">
         <v>-77.038899999999998</v>
       </c>
     </row>
@@ -2501,16 +2508,16 @@
       <c r="A60" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D60" s="4">
+      <c r="D60" s="5">
         <v>-10.548299999999999</v>
       </c>
-      <c r="E60" s="4">
+      <c r="E60" s="5">
         <v>-77.112799999999993</v>
       </c>
     </row>
@@ -2518,16 +2525,16 @@
       <c r="A61" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D61" s="4">
+      <c r="D61" s="5">
         <v>-10.5953</v>
       </c>
-      <c r="E61" s="4">
+      <c r="E61" s="5">
         <v>-77.166899999999998</v>
       </c>
     </row>
@@ -2535,16 +2542,16 @@
       <c r="A62" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D62" s="5">
         <v>-11.467499999999999</v>
       </c>
-      <c r="E62" s="4">
+      <c r="E62" s="5">
         <v>-76.623099999999994</v>
       </c>
     </row>
@@ -2552,16 +2559,16 @@
       <c r="A63" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C63" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D63" s="4">
+      <c r="D63" s="5">
         <v>-11.622199999999999</v>
       </c>
-      <c r="E63" s="4">
+      <c r="E63" s="5">
         <v>-76.673100000000005</v>
       </c>
     </row>
@@ -2569,16 +2576,16 @@
       <c r="A64" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D64" s="4">
+      <c r="D64" s="5">
         <v>-11.499700000000001</v>
       </c>
-      <c r="E64" s="4">
+      <c r="E64" s="5">
         <v>-76.748900000000006</v>
       </c>
     </row>
@@ -2586,16 +2593,16 @@
       <c r="A65" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C65" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D65" s="4">
+      <c r="D65" s="5">
         <v>-11.405799999999999</v>
       </c>
-      <c r="E65" s="4">
+      <c r="E65" s="5">
         <v>-76.576099999999997</v>
       </c>
     </row>
@@ -2603,16 +2610,16 @@
       <c r="A66" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D66" s="4">
+      <c r="D66" s="5">
         <v>-11.556699999999999</v>
       </c>
-      <c r="E66" s="4">
+      <c r="E66" s="5">
         <v>-76.624399999999994</v>
       </c>
     </row>
@@ -2620,16 +2627,16 @@
       <c r="A67" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C67" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D67" s="4">
+      <c r="D67" s="5">
         <v>-11.489699999999999</v>
       </c>
-      <c r="E67" s="4">
+      <c r="E67" s="5">
         <v>-76.6631</v>
       </c>
     </row>
@@ -2637,16 +2644,16 @@
       <c r="A68" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C68" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D68" s="4">
+      <c r="D68" s="5">
         <v>-11.6928</v>
       </c>
-      <c r="E68" s="4">
+      <c r="E68" s="5">
         <v>-76.844399999999993</v>
       </c>
     </row>
@@ -2654,16 +2661,16 @@
       <c r="A69" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C69" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D69" s="4">
+      <c r="D69" s="5">
         <v>-13.0825</v>
       </c>
-      <c r="E69" s="4">
+      <c r="E69" s="5">
         <v>-76.388300000000001</v>
       </c>
     </row>
@@ -2671,16 +2678,16 @@
       <c r="A70" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C70" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D70" s="4">
+      <c r="D70" s="5">
         <v>-12.7789</v>
       </c>
-      <c r="E70" s="4">
+      <c r="E70" s="5">
         <v>-76.557199999999995</v>
       </c>
     </row>
@@ -2688,16 +2695,16 @@
       <c r="A71" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C71" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D71" s="4">
+      <c r="D71" s="5">
         <v>-12.525600000000001</v>
       </c>
-      <c r="E71" s="4">
+      <c r="E71" s="5">
         <v>-76.543300000000002</v>
       </c>
     </row>
@@ -2705,16 +2712,16 @@
       <c r="A72" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C72" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D72" s="4">
+      <c r="D72" s="5">
         <v>-13.0267</v>
       </c>
-      <c r="E72" s="4">
+      <c r="E72" s="5">
         <v>-76.479399999999998</v>
       </c>
     </row>
@@ -2722,16 +2729,16 @@
       <c r="A73" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C73" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D73" s="4">
+      <c r="D73" s="5">
         <v>-12.517200000000001</v>
       </c>
-      <c r="E73" s="4">
+      <c r="E73" s="5">
         <v>-76.736099999999993</v>
       </c>
     </row>
@@ -2739,16 +2746,16 @@
       <c r="A74" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C74" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D74" s="4">
+      <c r="D74" s="5">
         <v>-12.7258</v>
       </c>
-      <c r="E74" s="4">
+      <c r="E74" s="5">
         <v>-76.460599999999999</v>
       </c>
     </row>
@@ -2756,16 +2763,16 @@
       <c r="A75" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="C75" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D75" s="4">
+      <c r="D75" s="5">
         <v>-13.0608</v>
       </c>
-      <c r="E75" s="4">
+      <c r="E75" s="5">
         <v>-76.349999999999994</v>
       </c>
     </row>
@@ -2773,16 +2780,16 @@
       <c r="A76" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="C76" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D76" s="4">
+      <c r="D76" s="5">
         <v>-12.9597</v>
       </c>
-      <c r="E76" s="4">
+      <c r="E76" s="5">
         <v>-76.139200000000002</v>
       </c>
     </row>
@@ -2790,16 +2797,16 @@
       <c r="A77" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C77" s="4" t="s">
+      <c r="C77" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D77" s="4">
+      <c r="D77" s="5">
         <v>-12.6553</v>
       </c>
-      <c r="E77" s="4">
+      <c r="E77" s="5">
         <v>-76.63</v>
       </c>
     </row>
@@ -2807,16 +2814,16 @@
       <c r="A78" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C78" s="4" t="s">
+      <c r="C78" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D78" s="4">
+      <c r="D78" s="5">
         <v>-13.074199999999999</v>
       </c>
-      <c r="E78" s="4">
+      <c r="E78" s="5">
         <v>-76.315799999999996</v>
       </c>
     </row>
@@ -2824,16 +2831,16 @@
       <c r="A79" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C79" s="4" t="s">
+      <c r="C79" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D79" s="4">
+      <c r="D79" s="5">
         <v>-12.8636</v>
       </c>
-      <c r="E79" s="4">
+      <c r="E79" s="5">
         <v>-76.051900000000003</v>
       </c>
     </row>
@@ -2841,16 +2848,16 @@
       <c r="A80" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C80" s="4" t="s">
+      <c r="C80" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D80" s="4">
+      <c r="D80" s="5">
         <v>-12.95</v>
       </c>
-      <c r="E80" s="4">
+      <c r="E80" s="5">
         <v>-76.382800000000003</v>
       </c>
     </row>
@@ -2858,16 +2865,16 @@
       <c r="A81" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C81" s="4" t="s">
+      <c r="C81" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D81" s="4">
+      <c r="D81" s="5">
         <v>-12.6431</v>
       </c>
-      <c r="E81" s="4">
+      <c r="E81" s="5">
         <v>-76.650000000000006</v>
       </c>
     </row>
@@ -2875,16 +2882,16 @@
       <c r="A82" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="C82" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D82" s="4">
+      <c r="D82" s="5">
         <v>-13.050800000000001</v>
       </c>
-      <c r="E82" s="4">
+      <c r="E82" s="5">
         <v>-76.429400000000001</v>
       </c>
     </row>
@@ -2892,16 +2899,16 @@
       <c r="A83" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C83" s="4" t="s">
+      <c r="C83" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D83" s="4">
+      <c r="D83" s="5">
         <v>-12.619400000000001</v>
       </c>
-      <c r="E83" s="4">
+      <c r="E83" s="5">
         <v>-76.639700000000005</v>
       </c>
     </row>
@@ -2909,16 +2916,16 @@
       <c r="A84" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="C84" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D84" s="4">
+      <c r="D84" s="5">
         <v>-12.8581</v>
       </c>
-      <c r="E84" s="4">
+      <c r="E84" s="5">
         <v>-76.022499999999994</v>
       </c>
     </row>
@@ -2926,16 +2933,16 @@
       <c r="A85" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C85" s="4" t="s">
+      <c r="C85" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D85" s="4">
+      <c r="D85" s="5">
         <v>-11.491400000000001</v>
       </c>
-      <c r="E85" s="4">
+      <c r="E85" s="5">
         <v>-77.205299999999994</v>
       </c>
     </row>
@@ -2943,16 +2950,16 @@
       <c r="A86" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="C86" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D86" s="4">
+      <c r="D86" s="5">
         <v>-11.2331</v>
       </c>
-      <c r="E86" s="4">
+      <c r="E86" s="5">
         <v>-76.656099999999995</v>
       </c>
     </row>
@@ -2960,16 +2967,16 @@
       <c r="A87" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C87" s="4" t="s">
+      <c r="C87" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D87" s="4">
+      <c r="D87" s="5">
         <v>-11.353300000000001</v>
       </c>
-      <c r="E87" s="4">
+      <c r="E87" s="5">
         <v>-76.823099999999997</v>
       </c>
     </row>
@@ -2977,16 +2984,16 @@
       <c r="A88" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B88" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C88" s="4" t="s">
+      <c r="C88" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D88" s="4">
+      <c r="D88" s="5">
         <v>-11.559200000000001</v>
       </c>
-      <c r="E88" s="4">
+      <c r="E88" s="5">
         <v>-77.174400000000006</v>
       </c>
     </row>
@@ -2994,16 +3001,16 @@
       <c r="A89" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="C89" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D89" s="4">
+      <c r="D89" s="5">
         <v>-11.5669</v>
       </c>
-      <c r="E89" s="4">
+      <c r="E89" s="5">
         <v>-77.265799999999999</v>
       </c>
     </row>
@@ -3011,16 +3018,16 @@
       <c r="A90" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B90" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="C90" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D90" s="4">
+      <c r="D90" s="5">
         <v>-11.1889</v>
       </c>
-      <c r="E90" s="4">
+      <c r="E90" s="5">
         <v>-76.951899999999995</v>
       </c>
     </row>
@@ -3028,16 +3035,16 @@
       <c r="A91" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B91" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C91" s="4" t="s">
+      <c r="C91" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D91" s="4">
+      <c r="D91" s="5">
         <v>-11.2369</v>
       </c>
-      <c r="E91" s="4">
+      <c r="E91" s="5">
         <v>-76.8386</v>
       </c>
     </row>
@@ -3045,16 +3052,16 @@
       <c r="A92" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B92" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C92" s="4" t="s">
+      <c r="C92" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D92" s="4">
+      <c r="D92" s="5">
         <v>-11.183299999999999</v>
       </c>
-      <c r="E92" s="4">
+      <c r="E92" s="5">
         <v>-76.6464</v>
       </c>
     </row>
@@ -3062,16 +3069,16 @@
       <c r="A93" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B93" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C93" s="4" t="s">
+      <c r="C93" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D93" s="4">
+      <c r="D93" s="5">
         <v>-11.2736</v>
       </c>
-      <c r="E93" s="4">
+      <c r="E93" s="5">
         <v>-76.821399999999997</v>
       </c>
     </row>
@@ -3079,16 +3086,16 @@
       <c r="A94" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B94" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="C94" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D94" s="4">
+      <c r="D94" s="5">
         <v>-11.194699999999999</v>
       </c>
-      <c r="E94" s="4">
+      <c r="E94" s="5">
         <v>-76.633600000000001</v>
       </c>
     </row>
@@ -3096,16 +3103,16 @@
       <c r="A95" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B95" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C95" s="4" t="s">
+      <c r="C95" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D95" s="4">
+      <c r="D95" s="5">
         <v>-11.4072</v>
       </c>
-      <c r="E95" s="4">
+      <c r="E95" s="5">
         <v>-76.819400000000002</v>
       </c>
     </row>
@@ -3113,16 +3120,16 @@
       <c r="A96" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="C96" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D96" s="4">
+      <c r="D96" s="5">
         <v>-11.1919</v>
       </c>
-      <c r="E96" s="4">
+      <c r="E96" s="5">
         <v>-76.778599999999997</v>
       </c>
     </row>
@@ -3130,16 +3137,16 @@
       <c r="A97" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B97" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C97" s="4" t="s">
+      <c r="C97" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D97" s="4">
+      <c r="D97" s="5">
         <v>-11.845800000000001</v>
       </c>
-      <c r="E97" s="4">
+      <c r="E97" s="5">
         <v>-76.387799999999999</v>
       </c>
     </row>
@@ -3147,16 +3154,16 @@
       <c r="A98" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B98" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C98" s="4" t="s">
+      <c r="C98" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D98" s="4">
+      <c r="D98" s="5">
         <v>-12.0814</v>
       </c>
-      <c r="E98" s="4">
+      <c r="E98" s="5">
         <v>-76.513300000000001</v>
       </c>
     </row>
@@ -3164,16 +3171,16 @@
       <c r="A99" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B99" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C99" s="4" t="s">
+      <c r="C99" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D99" s="4">
+      <c r="D99" s="5">
         <v>-11.827500000000001</v>
       </c>
-      <c r="E99" s="4">
+      <c r="E99" s="5">
         <v>-76.6203</v>
       </c>
     </row>
@@ -3181,16 +3188,16 @@
       <c r="A100" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B100" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C100" s="4" t="s">
+      <c r="C100" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D100" s="4">
+      <c r="D100" s="5">
         <v>-11.6561</v>
       </c>
-      <c r="E100" s="4">
+      <c r="E100" s="5">
         <v>-76.518100000000004</v>
       </c>
     </row>
@@ -3198,16 +3205,16 @@
       <c r="A101" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B101" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C101" s="4" t="s">
+      <c r="C101" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D101" s="4">
+      <c r="D101" s="5">
         <v>-11.707800000000001</v>
       </c>
-      <c r="E101" s="4">
+      <c r="E101" s="5">
         <v>-76.271100000000004</v>
       </c>
     </row>
@@ -3215,16 +3222,16 @@
       <c r="A102" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B102" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C102" s="4" t="s">
+      <c r="C102" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D102" s="4">
+      <c r="D102" s="5">
         <v>-12.133599999999999</v>
       </c>
-      <c r="E102" s="4">
+      <c r="E102" s="5">
         <v>-76.437799999999996</v>
       </c>
     </row>
@@ -3232,16 +3239,16 @@
       <c r="A103" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B103" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C103" s="4" t="s">
+      <c r="C103" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D103" s="4">
+      <c r="D103" s="5">
         <v>-11.722799999999999</v>
       </c>
-      <c r="E103" s="4">
+      <c r="E103" s="5">
         <v>-76.59</v>
       </c>
     </row>
@@ -3249,16 +3256,16 @@
       <c r="A104" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B104" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C104" s="4" t="s">
+      <c r="C104" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D104" s="4">
+      <c r="D104" s="5">
         <v>-11.6561</v>
       </c>
-      <c r="E104" s="4">
+      <c r="E104" s="5">
         <v>-76.506900000000002</v>
       </c>
     </row>
@@ -3266,16 +3273,16 @@
       <c r="A105" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B105" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C105" s="4" t="s">
+      <c r="C105" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D105" s="4">
+      <c r="D105" s="5">
         <v>-12.1381</v>
       </c>
-      <c r="E105" s="4">
+      <c r="E105" s="5">
         <v>-76.234399999999994</v>
       </c>
     </row>
@@ -3283,16 +3290,16 @@
       <c r="A106" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B106" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C106" s="4" t="s">
+      <c r="C106" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D106" s="4">
+      <c r="D106" s="5">
         <v>-12.0969</v>
       </c>
-      <c r="E106" s="4">
+      <c r="E106" s="5">
         <v>-76.391099999999994</v>
       </c>
     </row>
@@ -3300,16 +3307,16 @@
       <c r="A107" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B107" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C107" s="4" t="s">
+      <c r="C107" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D107" s="4">
+      <c r="D107" s="5">
         <v>-12.125299999999999</v>
       </c>
-      <c r="E107" s="4">
+      <c r="E107" s="5">
         <v>-76.423299999999998</v>
       </c>
     </row>
@@ -3317,16 +3324,16 @@
       <c r="A108" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B108" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C108" s="4" t="s">
+      <c r="C108" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D108" s="4">
+      <c r="D108" s="5">
         <v>-11.6647</v>
       </c>
-      <c r="E108" s="4">
+      <c r="E108" s="5">
         <v>-76.542199999999994</v>
       </c>
     </row>
@@ -3334,16 +3341,16 @@
       <c r="A109" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B109" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C109" s="4" t="s">
+      <c r="C109" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D109" s="4">
+      <c r="D109" s="5">
         <v>-12.2378</v>
       </c>
-      <c r="E109" s="4">
+      <c r="E109" s="5">
         <v>-76.326099999999997</v>
       </c>
     </row>
@@ -3351,16 +3358,16 @@
       <c r="A110" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B110" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C110" s="4" t="s">
+      <c r="C110" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D110" s="4">
+      <c r="D110" s="5">
         <v>-11.925000000000001</v>
       </c>
-      <c r="E110" s="4">
+      <c r="E110" s="5">
         <v>-76.661699999999996</v>
       </c>
     </row>
@@ -3368,16 +3375,16 @@
       <c r="A111" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B111" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C111" s="4" t="s">
+      <c r="C111" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D111" s="4">
+      <c r="D111" s="5">
         <v>-12.0008</v>
       </c>
-      <c r="E111" s="4">
+      <c r="E111" s="5">
         <v>-76.477800000000002</v>
       </c>
     </row>
@@ -3385,16 +3392,16 @@
       <c r="A112" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B112" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C112" s="4" t="s">
+      <c r="C112" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D112" s="4">
+      <c r="D112" s="5">
         <v>-11.7439</v>
       </c>
-      <c r="E112" s="4">
+      <c r="E112" s="5">
         <v>-76.651899999999998</v>
       </c>
     </row>
@@ -3402,16 +3409,16 @@
       <c r="A113" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B113" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C113" s="4" t="s">
+      <c r="C113" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D113" s="4">
+      <c r="D113" s="5">
         <v>-11.9114</v>
       </c>
-      <c r="E113" s="4">
+      <c r="E113" s="5">
         <v>-76.527500000000003</v>
       </c>
     </row>
@@ -3419,16 +3426,16 @@
       <c r="A114" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B114" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C114" s="4" t="s">
+      <c r="C114" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D114" s="4">
+      <c r="D114" s="5">
         <v>-12.017799999999999</v>
       </c>
-      <c r="E114" s="4">
+      <c r="E114" s="5">
         <v>-76.393600000000006</v>
       </c>
     </row>
@@ -3436,16 +3443,16 @@
       <c r="A115" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B115" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C115" s="4" t="s">
+      <c r="C115" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D115" s="4">
+      <c r="D115" s="5">
         <v>-11.684699999999999</v>
       </c>
-      <c r="E115" s="4">
+      <c r="E115" s="5">
         <v>-76.527500000000003</v>
       </c>
     </row>
@@ -3453,16 +3460,16 @@
       <c r="A116" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B116" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C116" s="4" t="s">
+      <c r="C116" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D116" s="4">
+      <c r="D116" s="5">
         <v>-12.1136</v>
       </c>
-      <c r="E116" s="4">
+      <c r="E116" s="5">
         <v>-76.185000000000002</v>
       </c>
     </row>
@@ -3470,16 +3477,16 @@
       <c r="A117" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B117" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C117" s="4" t="s">
+      <c r="C117" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D117" s="4">
+      <c r="D117" s="5">
         <v>-12.145300000000001</v>
       </c>
-      <c r="E117" s="4">
+      <c r="E117" s="5">
         <v>-76.213300000000004</v>
       </c>
     </row>
@@ -3487,16 +3494,16 @@
       <c r="A118" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B118" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C118" s="4" t="s">
+      <c r="C118" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D118" s="4">
+      <c r="D118" s="5">
         <v>-11.758900000000001</v>
       </c>
-      <c r="E118" s="4">
+      <c r="E118" s="5">
         <v>-76.303100000000001</v>
       </c>
     </row>
@@ -3504,16 +3511,16 @@
       <c r="A119" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B119" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C119" s="4" t="s">
+      <c r="C119" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D119" s="4">
+      <c r="D119" s="5">
         <v>-11.868600000000001</v>
       </c>
-      <c r="E119" s="4">
+      <c r="E119" s="5">
         <v>-76.547499999999999</v>
       </c>
     </row>
@@ -3521,16 +3528,16 @@
       <c r="A120" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B120" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C120" s="4" t="s">
+      <c r="C120" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D120" s="4">
+      <c r="D120" s="5">
         <v>-11.7583</v>
       </c>
-      <c r="E120" s="4">
+      <c r="E120" s="5">
         <v>-76.5989</v>
       </c>
     </row>
@@ -3538,16 +3545,16 @@
       <c r="A121" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B121" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C121" s="4" t="s">
+      <c r="C121" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D121" s="4">
+      <c r="D121" s="5">
         <v>-12.1311</v>
       </c>
-      <c r="E121" s="4">
+      <c r="E121" s="5">
         <v>-76.218599999999995</v>
       </c>
     </row>
@@ -3555,16 +3562,16 @@
       <c r="A122" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B122" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C122" s="4" t="s">
+      <c r="C122" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D122" s="4">
+      <c r="D122" s="5">
         <v>-12.160600000000001</v>
       </c>
-      <c r="E122" s="4">
+      <c r="E122" s="5">
         <v>-76.229699999999994</v>
       </c>
     </row>
@@ -3572,16 +3579,16 @@
       <c r="A123" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B123" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C123" s="4" t="s">
+      <c r="C123" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D123" s="4">
+      <c r="D123" s="5">
         <v>-11.9108</v>
       </c>
-      <c r="E123" s="4">
+      <c r="E123" s="5">
         <v>-76.540599999999998</v>
       </c>
     </row>
@@ -3589,16 +3596,16 @@
       <c r="A124" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B124" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C124" s="4" t="s">
+      <c r="C124" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D124" s="4">
+      <c r="D124" s="5">
         <v>-11.910600000000001</v>
       </c>
-      <c r="E124" s="4">
+      <c r="E124" s="5">
         <v>-76.665599999999998</v>
       </c>
     </row>
@@ -3606,16 +3613,16 @@
       <c r="A125" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="B125" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C125" s="4" t="s">
+      <c r="C125" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D125" s="4">
+      <c r="D125" s="5">
         <v>-12.0961</v>
       </c>
-      <c r="E125" s="4">
+      <c r="E125" s="5">
         <v>-76.232500000000002</v>
       </c>
     </row>
@@ -3623,16 +3630,16 @@
       <c r="A126" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="B126" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C126" s="4" t="s">
+      <c r="C126" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D126" s="4">
+      <c r="D126" s="5">
         <v>-11.984999999999999</v>
       </c>
-      <c r="E126" s="4">
+      <c r="E126" s="5">
         <v>-76.527500000000003</v>
       </c>
     </row>
@@ -3640,16 +3647,16 @@
       <c r="A127" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B127" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C127" s="4" t="s">
+      <c r="C127" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D127" s="4">
+      <c r="D127" s="5">
         <v>-12.2203</v>
       </c>
-      <c r="E127" s="4">
+      <c r="E127" s="5">
         <v>-76.516099999999994</v>
       </c>
     </row>
@@ -3657,16 +3664,16 @@
       <c r="A128" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B128" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C128" s="4" t="s">
+      <c r="C128" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D128" s="4">
+      <c r="D128" s="5">
         <v>-11.885</v>
       </c>
-      <c r="E128" s="4">
+      <c r="E128" s="5">
         <v>-76.442499999999995</v>
       </c>
     </row>
@@ -3674,16 +3681,16 @@
       <c r="A129" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="B129" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C129" s="4" t="s">
+      <c r="C129" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D129" s="4">
+      <c r="D129" s="5">
         <v>-11.1069</v>
       </c>
-      <c r="E129" s="4">
+      <c r="E129" s="5">
         <v>-77.61</v>
       </c>
     </row>
@@ -3691,16 +3698,16 @@
       <c r="A130" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="B130" s="4" t="s">
+      <c r="B130" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C130" s="4" t="s">
+      <c r="C130" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D130" s="4">
+      <c r="D130" s="5">
         <v>-10.757199999999999</v>
       </c>
-      <c r="E130" s="4">
+      <c r="E130" s="5">
         <v>-77.269400000000005</v>
       </c>
     </row>
@@ -3708,16 +3715,16 @@
       <c r="A131" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B131" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C131" s="4" t="s">
+      <c r="C131" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D131" s="4">
+      <c r="D131" s="5">
         <v>-11.091699999999999</v>
       </c>
-      <c r="E131" s="4">
+      <c r="E131" s="5">
         <v>-77.627799999999993</v>
       </c>
     </row>
@@ -3725,16 +3732,16 @@
       <c r="A132" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="B132" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C132" s="4" t="s">
+      <c r="C132" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D132" s="4">
+      <c r="D132" s="5">
         <v>-10.935</v>
       </c>
-      <c r="E132" s="4">
+      <c r="E132" s="5">
         <v>-76.833600000000004</v>
       </c>
     </row>
@@ -3742,16 +3749,16 @@
       <c r="A133" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B133" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C133" s="4" t="s">
+      <c r="C133" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D133" s="4">
+      <c r="D133" s="5">
         <v>-11.1014</v>
       </c>
-      <c r="E133" s="4">
+      <c r="E133" s="5">
         <v>-77.61</v>
       </c>
     </row>
@@ -3759,16 +3766,16 @@
       <c r="A134" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="B134" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C134" s="4" t="s">
+      <c r="C134" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D134" s="4">
+      <c r="D134" s="5">
         <v>-11.0692</v>
       </c>
-      <c r="E134" s="4">
+      <c r="E134" s="5">
         <v>-77.600300000000004</v>
       </c>
     </row>
@@ -3776,16 +3783,16 @@
       <c r="A135" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B135" s="4" t="s">
+      <c r="B135" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C135" s="4" t="s">
+      <c r="C135" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D135" s="4">
+      <c r="D135" s="5">
         <v>-11.0586</v>
       </c>
-      <c r="E135" s="4">
+      <c r="E135" s="5">
         <v>-76.930800000000005</v>
       </c>
     </row>
@@ -3793,16 +3800,16 @@
       <c r="A136" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="B136" s="4" t="s">
+      <c r="B136" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C136" s="4" t="s">
+      <c r="C136" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D136" s="4">
+      <c r="D136" s="5">
         <v>-10.9567</v>
       </c>
-      <c r="E136" s="4">
+      <c r="E136" s="5">
         <v>-76.933599999999998</v>
       </c>
     </row>
@@ -3810,16 +3817,16 @@
       <c r="A137" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="B137" s="4" t="s">
+      <c r="B137" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C137" s="4" t="s">
+      <c r="C137" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D137" s="4">
+      <c r="D137" s="5">
         <v>-10.9483</v>
       </c>
-      <c r="E137" s="4">
+      <c r="E137" s="5">
         <v>-76.744699999999995</v>
       </c>
     </row>
@@ -3827,16 +3834,16 @@
       <c r="A138" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B138" s="4" t="s">
+      <c r="B138" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C138" s="4" t="s">
+      <c r="C138" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D138" s="4">
+      <c r="D138" s="5">
         <v>-11.0883</v>
       </c>
-      <c r="E138" s="4">
+      <c r="E138" s="5">
         <v>-77.588300000000004</v>
       </c>
     </row>
@@ -3844,16 +3851,16 @@
       <c r="A139" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="B139" s="4" t="s">
+      <c r="B139" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C139" s="4" t="s">
+      <c r="C139" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D139" s="4">
+      <c r="D139" s="5">
         <v>-11.1364</v>
       </c>
-      <c r="E139" s="4">
+      <c r="E139" s="5">
         <v>-77.191699999999997</v>
       </c>
     </row>
@@ -3861,16 +3868,16 @@
       <c r="A140" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B140" s="4" t="s">
+      <c r="B140" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C140" s="4" t="s">
+      <c r="C140" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D140" s="4">
+      <c r="D140" s="5">
         <v>-11.022500000000001</v>
       </c>
-      <c r="E140" s="4">
+      <c r="E140" s="5">
         <v>-77.642499999999998</v>
       </c>
     </row>
@@ -3878,16 +3885,16 @@
       <c r="A141" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="B141" s="4" t="s">
+      <c r="B141" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C141" s="4" t="s">
+      <c r="C141" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D141" s="4">
+      <c r="D141" s="5">
         <v>-10.6692</v>
       </c>
-      <c r="E141" s="4">
+      <c r="E141" s="5">
         <v>-76.772800000000004</v>
       </c>
     </row>
@@ -3895,16 +3902,16 @@
       <c r="A142" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="B142" s="4" t="s">
+      <c r="B142" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C142" s="4" t="s">
+      <c r="C142" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D142" s="4">
+      <c r="D142" s="5">
         <v>-10.791399999999999</v>
       </c>
-      <c r="E142" s="4">
+      <c r="E142" s="5">
         <v>-76.91</v>
       </c>
     </row>
@@ -3912,16 +3919,16 @@
       <c r="A143" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="B143" s="4" t="s">
+      <c r="B143" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C143" s="4" t="s">
+      <c r="C143" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D143" s="4">
+      <c r="D143" s="5">
         <v>-10.805300000000001</v>
       </c>
-      <c r="E143" s="4">
+      <c r="E143" s="5">
         <v>-76.9786</v>
       </c>
     </row>
@@ -3929,16 +3936,16 @@
       <c r="A144" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B144" s="4" t="s">
+      <c r="B144" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C144" s="4" t="s">
+      <c r="C144" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D144" s="4">
+      <c r="D144" s="5">
         <v>-10.861700000000001</v>
       </c>
-      <c r="E144" s="4">
+      <c r="E144" s="5">
         <v>-77.127799999999993</v>
       </c>
     </row>
@@ -3946,16 +3953,16 @@
       <c r="A145" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="B145" s="4" t="s">
+      <c r="B145" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C145" s="4" t="s">
+      <c r="C145" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D145" s="4">
+      <c r="D145" s="5">
         <v>-10.8353</v>
       </c>
-      <c r="E145" s="4">
+      <c r="E145" s="5">
         <v>-77.012200000000007</v>
       </c>
     </row>
@@ -3963,16 +3970,16 @@
       <c r="A146" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B146" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C146" s="4" t="s">
+      <c r="C146" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D146" s="4">
+      <c r="D146" s="5">
         <v>-10.8125</v>
       </c>
-      <c r="E146" s="4">
+      <c r="E146" s="5">
         <v>-76.874399999999994</v>
       </c>
     </row>
@@ -3980,16 +3987,16 @@
       <c r="A147" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B147" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C147" s="4" t="s">
+      <c r="C147" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D147" s="4">
+      <c r="D147" s="5">
         <v>-12.46</v>
       </c>
-      <c r="E147" s="4">
+      <c r="E147" s="5">
         <v>-75.921700000000001</v>
       </c>
     </row>
@@ -3997,16 +4004,16 @@
       <c r="A148" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="B148" s="4" t="s">
+      <c r="B148" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C148" s="4" t="s">
+      <c r="C148" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D148" s="4">
+      <c r="D148" s="5">
         <v>-12.2803</v>
       </c>
-      <c r="E148" s="4">
+      <c r="E148" s="5">
         <v>-75.7864</v>
       </c>
     </row>
@@ -4014,16 +4021,16 @@
       <c r="A149" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="B149" s="4" t="s">
+      <c r="B149" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C149" s="4" t="s">
+      <c r="C149" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D149" s="4">
+      <c r="D149" s="5">
         <v>-12.5922</v>
       </c>
-      <c r="E149" s="4">
+      <c r="E149" s="5">
         <v>-76.036699999999996</v>
       </c>
     </row>
@@ -4031,16 +4038,16 @@
       <c r="A150" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="B150" s="4" t="s">
+      <c r="B150" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C150" s="4" t="s">
+      <c r="C150" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D150" s="4">
+      <c r="D150" s="5">
         <v>-12.3825</v>
       </c>
-      <c r="E150" s="4">
+      <c r="E150" s="5">
         <v>-76.138900000000007</v>
       </c>
     </row>
@@ -4048,16 +4055,16 @@
       <c r="A151" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="B151" s="4" t="s">
+      <c r="B151" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C151" s="4" t="s">
+      <c r="C151" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D151" s="4">
+      <c r="D151" s="5">
         <v>-12.9994</v>
       </c>
-      <c r="E151" s="4">
+      <c r="E151" s="5">
         <v>-75.836699999999993</v>
       </c>
     </row>
@@ -4065,16 +4072,16 @@
       <c r="A152" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="B152" s="4" t="s">
+      <c r="B152" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C152" s="4" t="s">
+      <c r="C152" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D152" s="4">
+      <c r="D152" s="5">
         <v>-12.8119</v>
       </c>
-      <c r="E152" s="4">
+      <c r="E152" s="5">
         <v>-75.782799999999995</v>
       </c>
     </row>
@@ -4082,16 +4089,16 @@
       <c r="A153" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="B153" s="4" t="s">
+      <c r="B153" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C153" s="4" t="s">
+      <c r="C153" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D153" s="4">
+      <c r="D153" s="5">
         <v>-12.3444</v>
       </c>
-      <c r="E153" s="4">
+      <c r="E153" s="5">
         <v>-75.871700000000004</v>
       </c>
     </row>
@@ -4099,16 +4106,16 @@
       <c r="A154" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="B154" s="4" t="s">
+      <c r="B154" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C154" s="4" t="s">
+      <c r="C154" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D154" s="4">
+      <c r="D154" s="5">
         <v>-12.8003</v>
       </c>
-      <c r="E154" s="4">
+      <c r="E154" s="5">
         <v>-75.891099999999994</v>
       </c>
     </row>
@@ -4116,16 +4123,16 @@
       <c r="A155" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="B155" s="4" t="s">
+      <c r="B155" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C155" s="4" t="s">
+      <c r="C155" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D155" s="4">
+      <c r="D155" s="5">
         <v>-12.9133</v>
       </c>
-      <c r="E155" s="4">
+      <c r="E155" s="5">
         <v>-75.863100000000003</v>
       </c>
     </row>
@@ -4133,16 +4140,16 @@
       <c r="A156" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="B156" s="4" t="s">
+      <c r="B156" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C156" s="4" t="s">
+      <c r="C156" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D156" s="4">
+      <c r="D156" s="5">
         <v>-12.2964</v>
       </c>
-      <c r="E156" s="4">
+      <c r="E156" s="5">
         <v>-76.158900000000003</v>
       </c>
     </row>
@@ -4150,16 +4157,16 @@
       <c r="A157" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B157" s="4" t="s">
+      <c r="B157" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C157" s="4" t="s">
+      <c r="C157" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D157" s="4">
+      <c r="D157" s="5">
         <v>-12.6319</v>
       </c>
-      <c r="E157" s="4">
+      <c r="E157" s="5">
         <v>-75.890600000000006</v>
       </c>
     </row>
@@ -4167,16 +4174,16 @@
       <c r="A158" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="B158" s="4" t="s">
+      <c r="B158" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C158" s="4" t="s">
+      <c r="C158" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D158" s="4">
+      <c r="D158" s="5">
         <v>-12.8108</v>
       </c>
-      <c r="E158" s="4">
+      <c r="E158" s="5">
         <v>-75.764700000000005</v>
       </c>
     </row>
@@ -4184,16 +4191,16 @@
       <c r="A159" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="B159" s="4" t="s">
+      <c r="B159" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C159" s="4" t="s">
+      <c r="C159" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D159" s="4">
+      <c r="D159" s="5">
         <v>-12.360799999999999</v>
       </c>
-      <c r="E159" s="4">
+      <c r="E159" s="5">
         <v>-76.1661</v>
       </c>
     </row>
@@ -4201,16 +4208,16 @@
       <c r="A160" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="B160" s="4" t="s">
+      <c r="B160" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C160" s="4" t="s">
+      <c r="C160" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D160" s="4">
+      <c r="D160" s="5">
         <v>-12.2028</v>
       </c>
-      <c r="E160" s="4">
+      <c r="E160" s="5">
         <v>-75.799199999999999</v>
       </c>
     </row>
@@ -4218,16 +4225,16 @@
       <c r="A161" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="B161" s="4" t="s">
+      <c r="B161" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C161" s="4" t="s">
+      <c r="C161" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D161" s="4">
+      <c r="D161" s="5">
         <v>-12.899699999999999</v>
       </c>
-      <c r="E161" s="4">
+      <c r="E161" s="5">
         <v>-75.831100000000006</v>
       </c>
     </row>
@@ -4235,16 +4242,16 @@
       <c r="A162" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="B162" s="4" t="s">
+      <c r="B162" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C162" s="4" t="s">
+      <c r="C162" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D162" s="4">
+      <c r="D162" s="5">
         <v>-12.4572</v>
       </c>
-      <c r="E162" s="4">
+      <c r="E162" s="5">
         <v>-75.810599999999994</v>
       </c>
     </row>
@@ -4252,16 +4259,16 @@
       <c r="A163" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="B163" s="4" t="s">
+      <c r="B163" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C163" s="4" t="s">
+      <c r="C163" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D163" s="4">
+      <c r="D163" s="5">
         <v>-12.293900000000001</v>
       </c>
-      <c r="E163" s="4">
+      <c r="E163" s="5">
         <v>-76.138599999999997</v>
       </c>
     </row>
@@ -4269,16 +4276,16 @@
       <c r="A164" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="B164" s="4" t="s">
+      <c r="B164" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C164" s="4" t="s">
+      <c r="C164" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D164" s="4">
+      <c r="D164" s="5">
         <v>-12.345599999999999</v>
       </c>
-      <c r="E164" s="4">
+      <c r="E164" s="5">
         <v>-75.785600000000002</v>
       </c>
     </row>
@@ -4286,16 +4293,16 @@
       <c r="A165" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="B165" s="4" t="s">
+      <c r="B165" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C165" s="4" t="s">
+      <c r="C165" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D165" s="4">
+      <c r="D165" s="5">
         <v>-12.8</v>
       </c>
-      <c r="E165" s="4">
+      <c r="E165" s="5">
         <v>-75.665800000000004</v>
       </c>
     </row>
@@ -4303,16 +4310,16 @@
       <c r="A166" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="B166" s="4" t="s">
+      <c r="B166" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C166" s="4" t="s">
+      <c r="C166" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D166" s="4">
+      <c r="D166" s="5">
         <v>-12.945</v>
       </c>
-      <c r="E166" s="4">
+      <c r="E166" s="5">
         <v>-75.777500000000003</v>
       </c>
     </row>
@@ -4320,16 +4327,16 @@
       <c r="A167" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="B167" s="4" t="s">
+      <c r="B167" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C167" s="4" t="s">
+      <c r="C167" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D167" s="4">
+      <c r="D167" s="5">
         <v>-12.274699999999999</v>
       </c>
-      <c r="E167" s="4">
+      <c r="E167" s="5">
         <v>-75.8536</v>
       </c>
     </row>
@@ -4337,16 +4344,16 @@
       <c r="A168" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="B168" s="4" t="s">
+      <c r="B168" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C168" s="4" t="s">
+      <c r="C168" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D168" s="4">
+      <c r="D168" s="5">
         <v>-12.517200000000001</v>
       </c>
-      <c r="E168" s="4">
+      <c r="E168" s="5">
         <v>-76.290300000000002</v>
       </c>
     </row>
@@ -4354,16 +4361,16 @@
       <c r="A169" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="B169" s="4" t="s">
+      <c r="B169" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C169" s="4" t="s">
+      <c r="C169" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D169" s="4">
+      <c r="D169" s="5">
         <v>-12.668900000000001</v>
       </c>
-      <c r="E169" s="4">
+      <c r="E169" s="5">
         <v>-75.949399999999997</v>
       </c>
     </row>
@@ -4371,16 +4378,16 @@
       <c r="A170" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="B170" s="4" t="s">
+      <c r="B170" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C170" s="4" t="s">
+      <c r="C170" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D170" s="4">
+      <c r="D170" s="5">
         <v>-12.307499999999999</v>
       </c>
-      <c r="E170" s="4">
+      <c r="E170" s="5">
         <v>-76.142200000000003</v>
       </c>
     </row>
@@ -4388,16 +4395,16 @@
       <c r="A171" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="B171" s="4" t="s">
+      <c r="B171" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C171" s="4" t="s">
+      <c r="C171" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D171" s="4">
+      <c r="D171" s="5">
         <v>-12.3642</v>
       </c>
-      <c r="E171" s="4">
+      <c r="E171" s="5">
         <v>-76.226399999999998</v>
       </c>
     </row>
@@ -4405,16 +4412,16 @@
       <c r="A172" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B172" s="4" t="s">
+      <c r="B172" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C172" s="4" t="s">
+      <c r="C172" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D172" s="4">
+      <c r="D172" s="5">
         <v>-12.2844</v>
       </c>
-      <c r="E172" s="4">
+      <c r="E172" s="5">
         <v>-76.1464</v>
       </c>
     </row>
@@ -4422,16 +4429,16 @@
       <c r="A173" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="B173" s="4" t="s">
+      <c r="B173" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C173" s="4" t="s">
+      <c r="C173" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D173" s="4">
+      <c r="D173" s="5">
         <v>-12.4544</v>
       </c>
-      <c r="E173" s="4">
+      <c r="E173" s="5">
         <v>-76.226699999999994</v>
       </c>
     </row>
@@ -4439,16 +4446,16 @@
       <c r="A174" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="B174" s="4" t="s">
+      <c r="B174" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C174" s="4" t="s">
+      <c r="C174" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D174" s="4">
+      <c r="D174" s="5">
         <v>-12.1214</v>
       </c>
-      <c r="E174" s="4">
+      <c r="E174" s="5">
         <v>-76.012200000000007</v>
       </c>
     </row>
@@ -4456,16 +4463,16 @@
       <c r="A175" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="B175" s="4" t="s">
+      <c r="B175" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C175" s="4" t="s">
+      <c r="C175" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D175" s="4">
+      <c r="D175" s="5">
         <v>-12.615600000000001</v>
       </c>
-      <c r="E175" s="4">
+      <c r="E175" s="5">
         <v>-76.16</v>
       </c>
     </row>
@@ -4473,16 +4480,16 @@
       <c r="A176" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B176" s="4" t="s">
+      <c r="B176" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C176" s="4" t="s">
+      <c r="C176" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D176" s="4">
+      <c r="D176" s="5">
         <v>-12.2372</v>
       </c>
-      <c r="E176" s="4">
+      <c r="E176" s="5">
         <v>-75.746099999999998</v>
       </c>
     </row>
@@ -4490,16 +4497,16 @@
       <c r="A177" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="B177" s="4" t="s">
+      <c r="B177" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C177" s="4" t="s">
+      <c r="C177" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D177" s="4">
+      <c r="D177" s="5">
         <v>-12.7403</v>
       </c>
-      <c r="E177" s="4">
+      <c r="E177" s="5">
         <v>-75.808899999999994</v>
       </c>
     </row>
@@ -4507,16 +4514,16 @@
       <c r="A178" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="B178" s="4" t="s">
+      <c r="B178" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C178" s="4" t="s">
+      <c r="C178" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D178" s="4">
+      <c r="D178" s="5">
         <v>-12.931100000000001</v>
       </c>
-      <c r="E178" s="4">
+      <c r="E178" s="5">
         <v>-75.779399999999995</v>
       </c>
     </row>
@@ -4524,16 +4531,16 @@
       <c r="A179" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="B179" s="4" t="s">
+      <c r="B179" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C179" s="4" t="s">
+      <c r="C179" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D179" s="4">
+      <c r="D179" s="5">
         <v>-12.223599999999999</v>
       </c>
-      <c r="E179" s="4">
+      <c r="E179" s="5">
         <v>-75.806899999999999</v>
       </c>
     </row>

</xml_diff>